<commit_message>
Adicionado logs no wf de acesso ao portal e download da fatura
</commit_message>
<xml_diff>
--- a/Data/Input/Relatório_Sintético.xlsx
+++ b/Data/Input/Relatório_Sintético.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <x:si>
     <x:t>.....</x:t>
   </x:si>
@@ -251,6 +251,15 @@
   </x:si>
   <x:si>
     <x:t>00:01:57</x:t>
+  </x:si>
+  <x:si>
+    <x:t>31/03/2022 12:28:56</x:t>
+  </x:si>
+  <x:si>
+    <x:t>31/03/2022 12:31:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00:02:04</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -403,8 +412,95 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="640">
+  <x:cellStyleXfs count="669">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="20" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="20" fontId="7" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -3302,11 +3398,21 @@
       </x:c>
     </x:row>
     <x:row r="28" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <x:c r="A28" s="7" t="s"/>
-      <x:c r="B28" s="3" t="s"/>
-      <x:c r="C28" s="3" t="s"/>
-      <x:c r="D28" s="11" t="s"/>
-      <x:c r="E28" s="6" t="s"/>
+      <x:c r="A28" s="7" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B28" s="3" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C28" s="3" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="D28" s="11" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="E28" s="6" t="s">
+        <x:v>44</x:v>
+      </x:c>
     </x:row>
     <x:row r="29" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <x:c r="A29" s="7" t="s"/>

</xml_diff>

<commit_message>
Add logs wf download.
</commit_message>
<xml_diff>
--- a/Data/Input/Relatório_Sintético.xlsx
+++ b/Data/Input/Relatório_Sintético.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <x:si>
     <x:t>.....</x:t>
   </x:si>
@@ -299,6 +299,24 @@
   </x:si>
   <x:si>
     <x:t>00:00:17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08/04/2022 17:49:54</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08/04/2022 17:52:13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00:02:18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08/04/2022 22:14:13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08/04/2022 22:15:59</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00:01:45</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -451,8 +469,182 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="785">
+  <x:cellStyleXfs count="843">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="20" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="20" fontId="7" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="20" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="20" fontId="7" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -3870,18 +4062,38 @@
       </x:c>
     </x:row>
     <x:row r="33" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <x:c r="A33" s="7" t="s"/>
-      <x:c r="B33" s="3" t="s"/>
-      <x:c r="C33" s="3" t="s"/>
-      <x:c r="D33" s="11" t="s"/>
-      <x:c r="E33" s="6" t="s"/>
+      <x:c r="A33" s="7" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B33" s="3" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="C33" s="3" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="D33" s="11" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="E33" s="6" t="s">
+        <x:v>13</x:v>
+      </x:c>
     </x:row>
     <x:row r="34" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <x:c r="A34" s="7" t="s"/>
-      <x:c r="B34" s="3" t="s"/>
-      <x:c r="C34" s="3" t="s"/>
-      <x:c r="D34" s="11" t="s"/>
-      <x:c r="E34" s="6" t="s"/>
+      <x:c r="A34" s="7" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B34" s="3" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="C34" s="3" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="D34" s="11" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="E34" s="6" t="s">
+        <x:v>44</x:v>
+      </x:c>
     </x:row>
     <x:row r="35" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <x:c r="A35" s="7" t="s"/>

</xml_diff>

<commit_message>
Add atividade de check e logs
</commit_message>
<xml_diff>
--- a/Data/Input/Relatório_Sintético.xlsx
+++ b/Data/Input/Relatório_Sintético.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <x:si>
     <x:t>.....</x:t>
   </x:si>
@@ -317,6 +317,15 @@
   </x:si>
   <x:si>
     <x:t>00:01:45</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11/04/2022 11:13:08</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11/04/2022 11:25:28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00:12:19</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -469,8 +478,95 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="843">
+  <x:cellStyleXfs count="872">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="20" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="20" fontId="7" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -4096,11 +4192,21 @@
       </x:c>
     </x:row>
     <x:row r="35" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <x:c r="A35" s="7" t="s"/>
-      <x:c r="B35" s="3" t="s"/>
-      <x:c r="C35" s="3" t="s"/>
-      <x:c r="D35" s="11" t="s"/>
-      <x:c r="E35" s="6" t="s"/>
+      <x:c r="A35" s="7" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B35" s="3" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="C35" s="3" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="D35" s="11" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="E35" s="6" t="s">
+        <x:v>87</x:v>
+      </x:c>
     </x:row>
     <x:row r="36" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <x:c r="A36" s="7" t="s"/>

</xml_diff>

<commit_message>
Ajustes no seletor wf de download
</commit_message>
<xml_diff>
--- a/Data/Input/Relatório_Sintético.xlsx
+++ b/Data/Input/Relatório_Sintético.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <x:si>
     <x:t>.....</x:t>
   </x:si>
@@ -326,6 +326,15 @@
   </x:si>
   <x:si>
     <x:t>00:12:19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19/04/2022 17:39:35</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19/04/2022 17:41:29</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00:01:54</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -478,8 +487,95 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="872">
+  <x:cellStyleXfs count="901">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="20" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="20" fontId="7" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -4209,11 +4305,21 @@
       </x:c>
     </x:row>
     <x:row r="36" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <x:c r="A36" s="7" t="s"/>
-      <x:c r="B36" s="3" t="s"/>
-      <x:c r="C36" s="3" t="s"/>
-      <x:c r="D36" s="11" t="s"/>
-      <x:c r="E36" s="6" t="s"/>
+      <x:c r="A36" s="7" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B36" s="3" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="C36" s="3" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="D36" s="11" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="E36" s="6" t="s">
+        <x:v>71</x:v>
+      </x:c>
     </x:row>
     <x:row r="37" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <x:c r="A37" s="7" t="s"/>

</xml_diff>